<commit_message>
verifying/cleaning data pre link
</commit_message>
<xml_diff>
--- a/data/schedule.xlsx
+++ b/data/schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohit.b.aggarwal/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohitaggarwal/gitroot/ethcc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD7DCBF-7FF7-9246-913B-717D8C63E172}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5942258-408A-0A48-9837-759AA08CF8AC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16460" xr2:uid="{2B9DBD48-4A57-3B45-863B-968DD97EAE30}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16420" xr2:uid="{2B9DBD48-4A57-3B45-863B-968DD97EAE30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -138,12 +138,6 @@
     <t>Infrastructure Services in the swarm</t>
   </si>
   <si>
-    <t>Gregor Zavcer</t>
-  </si>
-  <si>
-    <t>Viktor Tron</t>
-  </si>
-  <si>
     <t>Who owns you? The case for Linnia and Web 3.0</t>
   </si>
   <si>
@@ -183,9 +177,6 @@
     <t>Jared Wasinger</t>
   </si>
   <si>
-    <t>Pawel Bylica</t>
-  </si>
-  <si>
     <t>Hera: The eWASM VM</t>
   </si>
   <si>
@@ -195,9 +186,6 @@
     <t>KWASM: Overview and path to KWASM</t>
   </si>
   <si>
-    <t>Everett Hildebrandt</t>
-  </si>
-  <si>
     <t>Special</t>
   </si>
   <si>
@@ -234,9 +222,6 @@
     <t>Griefing oppurtunities in Kleros</t>
   </si>
   <si>
-    <t>Clemont Lesaege</t>
-  </si>
-  <si>
     <t>BlockID identity on ethereum</t>
   </si>
   <si>
@@ -267,9 +252,6 @@
     <t>Which governance for my tokens?</t>
   </si>
   <si>
-    <t>Philippe Hongiman</t>
-  </si>
-  <si>
     <t>Compliance Issues</t>
   </si>
   <si>
@@ -291,9 +273,6 @@
     <t>Regulatory framweork for blockchain payments</t>
   </si>
   <si>
-    <t>Xavier Lavayssiere</t>
-  </si>
-  <si>
     <t>Balanc3</t>
   </si>
   <si>
@@ -315,9 +294,6 @@
     <t>Ujo</t>
   </si>
   <si>
-    <t>Jack Spalone</t>
-  </si>
-  <si>
     <t>Dapp</t>
   </si>
   <si>
@@ -336,9 +312,6 @@
     <t>P2P Tech Workshop - Secure Scuttlebutt Introduction</t>
   </si>
   <si>
-    <t>Frankie Pangilnan</t>
-  </si>
-  <si>
     <t>Classrooms</t>
   </si>
   <si>
@@ -351,18 +324,12 @@
     <t>Next generation EVM Smart Fuzzer: Echidna</t>
   </si>
   <si>
-    <t>J.P. Smith</t>
-  </si>
-  <si>
     <t>Remix Workshop 1</t>
   </si>
   <si>
     <t>The Culture of Crypto Investing</t>
   </si>
   <si>
-    <t>Raine</t>
-  </si>
-  <si>
     <t>Tokens</t>
   </si>
   <si>
@@ -375,9 +342,6 @@
     <t>ERC 777 (token)</t>
   </si>
   <si>
-    <t>Jordi Bayline, Jacques Dafflon</t>
-  </si>
-  <si>
     <t>Parity</t>
   </si>
   <si>
@@ -639,9 +603,6 @@
     <t>Manticore, EVM symbolic execution engine</t>
   </si>
   <si>
-    <t>Josselin Feist, J.P. Smith</t>
-  </si>
-  <si>
     <t>Introduction to Game Theory for Blockchain</t>
   </si>
   <si>
@@ -681,9 +642,6 @@
     <t>Scalable Spanking</t>
   </si>
   <si>
-    <t>Ameen</t>
-  </si>
-  <si>
     <t>Raiden and State Channels</t>
   </si>
   <si>
@@ -835,6 +793,48 @@
   </si>
   <si>
     <t>Smart Contract Hacking</t>
+  </si>
+  <si>
+    <t>Gregor Žavcer</t>
+  </si>
+  <si>
+    <t>Viktor Trón</t>
+  </si>
+  <si>
+    <t>Paweł Bylica</t>
+  </si>
+  <si>
+    <t>Everett Hildenbrandt</t>
+  </si>
+  <si>
+    <t>Clément Lesaege</t>
+  </si>
+  <si>
+    <t>Philippe Honigman</t>
+  </si>
+  <si>
+    <t>Xavier Lavayssière</t>
+  </si>
+  <si>
+    <t>Jack Spallone</t>
+  </si>
+  <si>
+    <t>Frankie Pangilinan</t>
+  </si>
+  <si>
+    <t>JP Smith</t>
+  </si>
+  <si>
+    <t>Josselin Feist, JP Smith</t>
+  </si>
+  <si>
+    <t>Raine Revere</t>
+  </si>
+  <si>
+    <t>Jordi Baylina, Jacques Dafflon</t>
+  </si>
+  <si>
+    <t>Ameen Soleimani</t>
   </si>
 </sst>
 </file>
@@ -1195,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928AFEA8-7390-9743-9CB0-D0CF1E80B2DC}">
   <dimension ref="A1:I124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="G125" sqref="G125"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1233,7 +1233,7 @@
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1451,7 +1451,7 @@
         <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>256</v>
       </c>
       <c r="C11" t="s">
         <v>33</v>
@@ -1474,7 +1474,7 @@
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>257</v>
       </c>
       <c r="C12" t="s">
         <v>33</v>
@@ -1494,10 +1494,10 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
         <v>33</v>
@@ -1517,10 +1517,10 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
         <v>33</v>
@@ -1540,10 +1540,10 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
         <v>33</v>
@@ -1563,10 +1563,10 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
         <v>33</v>
@@ -1586,10 +1586,10 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
         <v>33</v>
@@ -1609,10 +1609,10 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
         <v>49</v>
-      </c>
-      <c r="B18" t="s">
-        <v>51</v>
       </c>
       <c r="C18" t="s">
         <v>33</v>
@@ -1632,10 +1632,10 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>258</v>
       </c>
       <c r="C19" t="s">
         <v>33</v>
@@ -1655,10 +1655,10 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
         <v>33</v>
@@ -1678,10 +1678,10 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>259</v>
       </c>
       <c r="C21" t="s">
         <v>33</v>
@@ -1701,10 +1701,10 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D22" s="2">
         <v>0.70138888888888884</v>
@@ -1719,18 +1719,18 @@
         <v>17</v>
       </c>
       <c r="I22" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D23" s="2">
         <v>0.38194444444444442</v>
@@ -1747,13 +1747,13 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D24" s="2">
         <v>0.40277777777777773</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D25" s="2">
         <v>0.45833333333333331</v>
@@ -1793,13 +1793,13 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>260</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D26" s="2">
         <v>0.47916666666666669</v>
@@ -1816,13 +1816,13 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D27" s="2">
         <v>0.58333333333333337</v>
@@ -1834,18 +1834,18 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D28" s="2">
         <v>0.59722222222222221</v>
@@ -1857,18 +1857,18 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D29" s="2">
         <v>0.61805555555555558</v>
@@ -1880,15 +1880,15 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C30" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D30" s="2">
         <v>0.63888888888888895</v>
@@ -1900,21 +1900,21 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="I30" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>261</v>
       </c>
       <c r="C31" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D31" s="2">
         <v>0.70833333333333337</v>
@@ -1931,13 +1931,13 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C32" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D32" s="2">
         <v>0.3923611111111111</v>
@@ -1949,18 +1949,18 @@
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D33" s="2">
         <v>0.41319444444444442</v>
@@ -1972,18 +1972,18 @@
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>262</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D34" s="2">
         <v>0.46180555555555558</v>
@@ -1995,18 +1995,18 @@
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C35" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D35" s="2">
         <v>0.4826388888888889</v>
@@ -2018,18 +2018,18 @@
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B36" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C36" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D36" s="2">
         <v>0.58680555555555558</v>
@@ -2046,13 +2046,13 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C37" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D37" s="2">
         <v>0.60763888888888895</v>
@@ -2069,13 +2069,13 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>263</v>
       </c>
       <c r="C38" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D38" s="2">
         <v>0.62847222222222221</v>
@@ -2087,18 +2087,18 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B39" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C39" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D39" s="2">
         <v>0.64930555555555558</v>
@@ -2110,18 +2110,18 @@
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B40" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C40" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D40" s="2">
         <v>0.70833333333333337</v>
@@ -2133,18 +2133,18 @@
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B41" t="s">
-        <v>103</v>
+        <v>264</v>
       </c>
       <c r="C41" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D41" s="2">
         <v>0.45833333333333331</v>
@@ -2156,15 +2156,15 @@
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C42" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D42" s="2">
         <v>0.47916666666666669</v>
@@ -2176,21 +2176,21 @@
         <v>0</v>
       </c>
       <c r="G42" t="s">
+        <v>89</v>
+      </c>
+      <c r="H42" t="s">
         <v>97</v>
-      </c>
-      <c r="H42" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B43" t="s">
-        <v>108</v>
+        <v>265</v>
       </c>
       <c r="C43" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D43" s="2">
         <v>0.58333333333333337</v>
@@ -2207,10 +2207,10 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C44" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D44" s="2">
         <v>0.6875</v>
@@ -2227,10 +2227,10 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>267</v>
       </c>
       <c r="C45" t="s">
         <v>10</v>
@@ -2245,15 +2245,15 @@
         <v>1</v>
       </c>
       <c r="G45" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B46" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C46" t="s">
         <v>10</v>
@@ -2268,15 +2268,15 @@
         <v>1</v>
       </c>
       <c r="G46" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
+        <v>268</v>
       </c>
       <c r="C47" t="s">
         <v>10</v>
@@ -2291,15 +2291,15 @@
         <v>1</v>
       </c>
       <c r="G47" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B48" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C48" t="s">
         <v>10</v>
@@ -2314,15 +2314,15 @@
         <v>1</v>
       </c>
       <c r="G48" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B49" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C49" t="s">
         <v>10</v>
@@ -2337,15 +2337,15 @@
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B50" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C50" t="s">
         <v>10</v>
@@ -2360,15 +2360,15 @@
         <v>1</v>
       </c>
       <c r="G50" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="B51" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C51" t="s">
         <v>10</v>
@@ -2383,15 +2383,15 @@
         <v>1</v>
       </c>
       <c r="G51" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B52" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C52" t="s">
         <v>10</v>
@@ -2406,15 +2406,15 @@
         <v>1</v>
       </c>
       <c r="G52" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B53" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="C53" t="s">
         <v>10</v>
@@ -2429,15 +2429,15 @@
         <v>1</v>
       </c>
       <c r="G53" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="B54" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C54" t="s">
         <v>10</v>
@@ -2452,15 +2452,15 @@
         <v>1</v>
       </c>
       <c r="G54" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="B55" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C55" t="s">
         <v>10</v>
@@ -2475,15 +2475,15 @@
         <v>1</v>
       </c>
       <c r="G55" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="B56" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="C56" t="s">
         <v>33</v>
@@ -2498,15 +2498,15 @@
         <v>1</v>
       </c>
       <c r="G56" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B57" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C57" t="s">
         <v>33</v>
@@ -2521,15 +2521,15 @@
         <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B58" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C58" t="s">
         <v>33</v>
@@ -2544,15 +2544,15 @@
         <v>1</v>
       </c>
       <c r="G58" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="B59" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="C59" t="s">
         <v>33</v>
@@ -2567,15 +2567,15 @@
         <v>1</v>
       </c>
       <c r="G59" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B60" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C60" t="s">
         <v>33</v>
@@ -2590,15 +2590,15 @@
         <v>1</v>
       </c>
       <c r="G60" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B61" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C61" t="s">
         <v>33</v>
@@ -2613,15 +2613,15 @@
         <v>1</v>
       </c>
       <c r="G61" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="B62" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C62" t="s">
         <v>33</v>
@@ -2636,15 +2636,15 @@
         <v>1</v>
       </c>
       <c r="G62" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="B63" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C63" t="s">
         <v>33</v>
@@ -2659,15 +2659,15 @@
         <v>1</v>
       </c>
       <c r="G63" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="B64" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C64" t="s">
         <v>33</v>
@@ -2682,15 +2682,15 @@
         <v>1</v>
       </c>
       <c r="G64" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="B65" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C65" t="s">
         <v>33</v>
@@ -2705,15 +2705,15 @@
         <v>1</v>
       </c>
       <c r="G65" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="B66" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C66" t="s">
         <v>33</v>
@@ -2728,18 +2728,18 @@
         <v>1</v>
       </c>
       <c r="G66" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="B67" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C67" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D67" s="2">
         <v>0.375</v>
@@ -2751,18 +2751,18 @@
         <v>1</v>
       </c>
       <c r="G67" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="B68" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C68" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D68" s="2">
         <v>0.39583333333333331</v>
@@ -2774,18 +2774,18 @@
         <v>1</v>
       </c>
       <c r="G68" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B69" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="C69" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D69" s="2">
         <v>0.41666666666666669</v>
@@ -2797,18 +2797,18 @@
         <v>1</v>
       </c>
       <c r="G69" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="B70" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C70" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D70" s="2">
         <v>0.45833333333333331</v>
@@ -2820,18 +2820,18 @@
         <v>1</v>
       </c>
       <c r="G70" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B71" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C71" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D71" s="2">
         <v>0.47916666666666669</v>
@@ -2843,18 +2843,18 @@
         <v>1</v>
       </c>
       <c r="G71" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B72" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="C72" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D72" s="2">
         <v>0.59027777777777779</v>
@@ -2866,18 +2866,18 @@
         <v>1</v>
       </c>
       <c r="G72" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="B73" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="C73" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D73" s="2">
         <v>0.625</v>
@@ -2889,18 +2889,18 @@
         <v>1</v>
       </c>
       <c r="G73" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="B74" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="C74" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D74" s="2">
         <v>0.64583333333333337</v>
@@ -2917,13 +2917,13 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="B75" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="C75" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D75" s="2">
         <v>0.70138888888888884</v>
@@ -2935,18 +2935,18 @@
         <v>1</v>
       </c>
       <c r="G75" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="B76" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="C76" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D76" s="2">
         <v>0.375</v>
@@ -2958,18 +2958,18 @@
         <v>1</v>
       </c>
       <c r="G76" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="B77" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="C77" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D77" s="2">
         <v>0.3888888888888889</v>
@@ -2981,18 +2981,18 @@
         <v>1</v>
       </c>
       <c r="G77" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="B78" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C78" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D78" s="2">
         <v>0.40972222222222227</v>
@@ -3004,18 +3004,18 @@
         <v>1</v>
       </c>
       <c r="G78" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="B79" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C79" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D79" s="2">
         <v>0.4513888888888889</v>
@@ -3027,18 +3027,18 @@
         <v>1</v>
       </c>
       <c r="G79" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="B80" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="C80" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D80" s="2">
         <v>0.47916666666666669</v>
@@ -3050,18 +3050,18 @@
         <v>1</v>
       </c>
       <c r="G80" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B81" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="C81" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D81" s="2">
         <v>0.5</v>
@@ -3073,15 +3073,15 @@
         <v>1</v>
       </c>
       <c r="G81" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="82" spans="1:8">
       <c r="A82" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="C82" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D82" s="2">
         <v>0.58333333333333337</v>
@@ -3096,18 +3096,18 @@
         <v>11</v>
       </c>
       <c r="H82" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="B83" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="C83" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D83" s="2">
         <v>0.60763888888888895</v>
@@ -3119,18 +3119,18 @@
         <v>1</v>
       </c>
       <c r="G83" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="B84" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="C84" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D84" s="2">
         <v>0.64583333333333337</v>
@@ -3142,18 +3142,18 @@
         <v>1</v>
       </c>
       <c r="G84" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="B85" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="C85" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D85" s="2">
         <v>0.66666666666666663</v>
@@ -3165,18 +3165,18 @@
         <v>1</v>
       </c>
       <c r="G85" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="86" spans="1:8">
       <c r="A86" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="B86" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="C86" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D86" s="2">
         <v>0.69097222222222221</v>
@@ -3193,13 +3193,13 @@
     </row>
     <row r="87" spans="1:8">
       <c r="A87" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="B87" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="C87" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D87" s="2">
         <v>0.375</v>
@@ -3211,18 +3211,18 @@
         <v>1</v>
       </c>
       <c r="G87" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="88" spans="1:8">
       <c r="A88" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="B88" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C88" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D88" s="2">
         <v>0.4375</v>
@@ -3234,18 +3234,18 @@
         <v>1</v>
       </c>
       <c r="G88" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="89" spans="1:8">
       <c r="A89" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="B89" t="s">
-        <v>204</v>
+        <v>266</v>
       </c>
       <c r="C89" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D89" s="2">
         <v>0.5625</v>
@@ -3262,13 +3262,13 @@
     </row>
     <row r="90" spans="1:8">
       <c r="A90" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="B90" t="s">
-        <v>69</v>
+        <v>260</v>
       </c>
       <c r="C90" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D90" s="2">
         <v>0.64583333333333337</v>
@@ -3280,15 +3280,15 @@
         <v>1</v>
       </c>
       <c r="G90" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="91" spans="1:8">
       <c r="A91" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="B91" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="C91" t="s">
         <v>10</v>
@@ -3303,15 +3303,15 @@
         <v>2</v>
       </c>
       <c r="G91" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="92" spans="1:8">
       <c r="A92" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="B92" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="C92" t="s">
         <v>10</v>
@@ -3326,15 +3326,15 @@
         <v>2</v>
       </c>
       <c r="G92" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="93" spans="1:8">
       <c r="A93" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="B93" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="C93" t="s">
         <v>10</v>
@@ -3349,15 +3349,15 @@
         <v>2</v>
       </c>
       <c r="G93" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="94" spans="1:8">
       <c r="A94" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="B94" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="C94" t="s">
         <v>10</v>
@@ -3372,15 +3372,15 @@
         <v>2</v>
       </c>
       <c r="G94" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="95" spans="1:8">
       <c r="A95" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="B95" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="C95" t="s">
         <v>10</v>
@@ -3395,15 +3395,15 @@
         <v>2</v>
       </c>
       <c r="G95" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="96" spans="1:8">
       <c r="A96" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="B96" t="s">
-        <v>218</v>
+        <v>269</v>
       </c>
       <c r="C96" t="s">
         <v>10</v>
@@ -3418,15 +3418,15 @@
         <v>2</v>
       </c>
       <c r="G96" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="97" spans="1:7">
       <c r="A97" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="B97" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C97" t="s">
         <v>10</v>
@@ -3441,15 +3441,15 @@
         <v>2</v>
       </c>
       <c r="G97" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="B98" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="C98" t="s">
         <v>10</v>
@@ -3464,15 +3464,15 @@
         <v>2</v>
       </c>
       <c r="G98" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="B99" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="C99" t="s">
         <v>10</v>
@@ -3487,15 +3487,15 @@
         <v>2</v>
       </c>
       <c r="G99" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="B100" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="C100" t="s">
         <v>10</v>
@@ -3510,15 +3510,15 @@
         <v>2</v>
       </c>
       <c r="G100" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="B101" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="C101" t="s">
         <v>33</v>
@@ -3533,15 +3533,15 @@
         <v>2</v>
       </c>
       <c r="G101" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="B102" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="C102" t="s">
         <v>33</v>
@@ -3556,15 +3556,15 @@
         <v>2</v>
       </c>
       <c r="G102" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B103" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="C103" t="s">
         <v>33</v>
@@ -3579,15 +3579,15 @@
         <v>2</v>
       </c>
       <c r="G103" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="B104" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="C104" t="s">
         <v>33</v>
@@ -3602,15 +3602,15 @@
         <v>2</v>
       </c>
       <c r="G104" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="B105" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="C105" t="s">
         <v>33</v>
@@ -3625,15 +3625,15 @@
         <v>2</v>
       </c>
       <c r="G105" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="B106" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="C106" t="s">
         <v>33</v>
@@ -3648,15 +3648,15 @@
         <v>2</v>
       </c>
       <c r="G106" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="B107" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="C107" t="s">
         <v>33</v>
@@ -3671,18 +3671,18 @@
         <v>2</v>
       </c>
       <c r="G107" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="B108" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="C108" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D108" s="2">
         <v>0.63541666666666663</v>
@@ -3694,18 +3694,18 @@
         <v>2</v>
       </c>
       <c r="G108" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="B109" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="C109" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D109" s="2">
         <v>0.375</v>
@@ -3717,18 +3717,18 @@
         <v>2</v>
       </c>
       <c r="G109" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="110" spans="1:7">
       <c r="A110" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="B110" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="C110" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D110" s="2">
         <v>0.40972222222222227</v>
@@ -3740,18 +3740,18 @@
         <v>2</v>
       </c>
       <c r="G110" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="B111" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="C111" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D111" s="2">
         <v>0.44444444444444442</v>
@@ -3763,18 +3763,18 @@
         <v>2</v>
       </c>
       <c r="G111" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="B112" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="C112" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D112" s="2">
         <v>0.46527777777777773</v>
@@ -3786,18 +3786,18 @@
         <v>2</v>
       </c>
       <c r="G112" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="113" spans="1:9">
       <c r="A113" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="B113" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="C113" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D113" s="2">
         <v>0.48958333333333331</v>
@@ -3809,18 +3809,18 @@
         <v>2</v>
       </c>
       <c r="G113" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="114" spans="1:9">
       <c r="A114" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="B114" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="C114" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D114" s="2">
         <v>0.58333333333333337</v>
@@ -3832,18 +3832,18 @@
         <v>2</v>
       </c>
       <c r="G114" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="115" spans="1:9">
       <c r="A115" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="B115" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="C115" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D115" s="2">
         <v>0.60416666666666663</v>
@@ -3855,18 +3855,18 @@
         <v>2</v>
       </c>
       <c r="G115" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="116" spans="1:9">
       <c r="A116" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="B116" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="C116" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D116" s="2">
         <v>0.62847222222222221</v>
@@ -3878,15 +3878,15 @@
         <v>2</v>
       </c>
       <c r="G116" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="C117" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D117" s="2">
         <v>0.64583333333333337</v>
@@ -3898,18 +3898,18 @@
         <v>2</v>
       </c>
       <c r="G117" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="118" spans="1:9">
       <c r="A118" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="B118" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="C118" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D118" s="2">
         <v>0.40277777777777773</v>
@@ -3921,18 +3921,18 @@
         <v>2</v>
       </c>
       <c r="G118" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="119" spans="1:9">
       <c r="A119" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="B119" t="s">
         <v>27</v>
       </c>
       <c r="C119" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D119" s="2">
         <v>0.4513888888888889</v>
@@ -3944,18 +3944,18 @@
         <v>2</v>
       </c>
       <c r="G119" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="120" spans="1:9">
       <c r="A120" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="B120" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="C120" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D120" s="2">
         <v>0.58333333333333337</v>
@@ -3967,15 +3967,15 @@
         <v>2</v>
       </c>
       <c r="G120" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="121" spans="1:9">
       <c r="A121" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="C121" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D121" s="2">
         <v>0.625</v>
@@ -3990,15 +3990,15 @@
         <v>11</v>
       </c>
       <c r="I121" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="122" spans="1:9">
       <c r="A122" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="C122" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D122" s="2">
         <v>0.375</v>
@@ -4010,18 +4010,18 @@
         <v>2</v>
       </c>
       <c r="G122" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="123" spans="1:9">
       <c r="A123" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="B123" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C123" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D123" s="2">
         <v>0.4375</v>
@@ -4033,18 +4033,18 @@
         <v>2</v>
       </c>
       <c r="G123" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="124" spans="1:9">
       <c r="A124" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="B124" t="s">
-        <v>69</v>
+        <v>260</v>
       </c>
       <c r="C124" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D124" s="2">
         <v>0.58333333333333337</v>
@@ -4056,7 +4056,7 @@
         <v>2</v>
       </c>
       <c r="G124" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>